<commit_message>
update checkpoint update subrepo
</commit_message>
<xml_diff>
--- a/Presentazione/costi.xlsx
+++ b/Presentazione/costi.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\SmartTrafficLight\Presentazione\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969D3159-3725-4782-8F3E-64D5A63C1E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADF8369-28D1-42A2-9989-8D740FBD8B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6344C2F7-7D87-4D74-BF02-F5F62C05BB84}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6344C2F7-7D87-4D74-BF02-F5F62C05BB84}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Antonio" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>telecamere</t>
   </si>
@@ -90,14 +91,39 @@
   </si>
   <si>
     <t>3500 - 4000</t>
+  </si>
+  <si>
+    <t>camera</t>
+  </si>
+  <si>
+    <t>installazione + materiale</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>singolo</t>
+  </si>
+  <si>
+    <t>modem</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>miniPC</t>
+  </si>
+  <si>
+    <t>scheda semaforo??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -128,9 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -447,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D467EF1-30BC-483F-95A8-284CE81A99CF}">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -609,4 +639,118 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07CD711-C63D-442B-8328-4CBB9661FCEA}">
+  <dimension ref="B1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <f>D2*C2</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>320</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <f>D3*C3</f>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2">
+        <v>150</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E6" si="0">D4*C4</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2">
+        <v>150</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2">
+        <v>500</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <f>SUM(E2:E7)</f>
+        <v>5080</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>